<commit_message>
pushing initial pass of revisions, still need a few things
</commit_message>
<xml_diff>
--- a/text/figures/table3_AJH.xlsx
+++ b/text/figures/table3_AJH.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10523"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adamhockenberry/Projects/ecoli_learning_bacterial_response_optimization/text/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adamhockenberry/Projects/ecoli_learning_bacterial_response_optimization/text/figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1128532A-8530-0543-BED6-1F9F6FF785FC}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D327FA4-A455-2C47-B627-A71E80F7C99E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="5460" windowWidth="28040" windowHeight="17440" xr2:uid="{4E2A6468-EC56-494A-AD41-30C4A785C514}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{4E2A6468-EC56-494A-AD41-30C4A785C514}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="23">
   <si>
     <t>A</t>
   </si>
@@ -81,14 +81,26 @@
     <t>B</t>
   </si>
   <si>
-    <t>Gluconate</t>
+    <t>base†</t>
+  </si>
+  <si>
+    <t>Stationary†</t>
+  </si>
+  <si>
+    <t>Gluconate***</t>
+  </si>
+  <si>
+    <t>Glucose***</t>
+  </si>
+  <si>
+    <t>high***</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -98,39 +110,27 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Helvetica"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Helvetica"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFB0007"/>
-      <name val="Helvetica"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="13"/>
       <color theme="1"/>
       <name val="Helvetica"/>
       <family val="2"/>
     </font>
     <font>
+      <b/>
       <sz val="12"/>
-      <color theme="4"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Helvetica"/>
       <family val="2"/>
     </font>
@@ -213,48 +213,39 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -574,7 +565,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="A1:E16"/>
+      <selection activeCell="E16" sqref="A11:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -585,28 +576,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>5</v>
       </c>
     </row>
@@ -617,8 +608,8 @@
       <c r="B3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>8</v>
+      <c r="C3" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>9</v>
@@ -634,11 +625,11 @@
       <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>9</v>
+      <c r="C4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>10</v>
@@ -648,11 +639,11 @@
       <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>8</v>
+      <c r="B5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>9</v>
@@ -679,35 +670,35 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="8" t="s">
+      <c r="B7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="13" t="s">
-        <v>15</v>
+      <c r="E7" s="7" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
     </row>
     <row r="10" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
@@ -719,7 +710,7 @@
       <c r="E10" s="10"/>
     </row>
     <row r="11" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B11" s="11" t="s">
@@ -745,8 +736,8 @@
       <c r="C12" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="6" t="s">
-        <v>18</v>
+      <c r="D12" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>10</v>
@@ -762,8 +753,8 @@
       <c r="C13" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="6" t="s">
-        <v>18</v>
+      <c r="D13" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>10</v>
@@ -804,24 +795,24 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="8" t="s">
+      <c r="B16" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="13" t="s">
-        <v>15</v>
+      <c r="E16" s="7" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="12"/>
+      <c r="A17" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>